<commit_message>
Refactor URI and finish reporting
</commit_message>
<xml_diff>
--- a/storage/jurnal-opex-2022.xlsx
+++ b/storage/jurnal-opex-2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2639">
   <si>
     <t>No ID</t>
   </si>
@@ -7596,250 +7596,343 @@
     <t>2022-09-22 09:20:24</t>
   </si>
   <si>
+    <t>2022-09-14</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 14/09/2022 pk 5097</t>
+  </si>
+  <si>
+    <t>2022-09-14/Normal/1663813479/M02PK5097</t>
+  </si>
+  <si>
+    <t>2022-09-22 09:24:39</t>
+  </si>
+  <si>
+    <t>2022-09-15</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 15/09/2022 pk 5086</t>
+  </si>
+  <si>
+    <t>2022-09-15/Normal/1663813592/M03PK5086</t>
+  </si>
+  <si>
+    <t>2022-09-22 09:26:32</t>
+  </si>
+  <si>
+    <t>2022-09-19</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 19/09/2022 pk 5090</t>
+  </si>
+  <si>
+    <t>2022-09-19/Normal/1663813725/M03PK5090</t>
+  </si>
+  <si>
+    <t>2022-09-22 09:28:45</t>
+  </si>
+  <si>
+    <t>2022-09-20</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 20/09/2022 pk 5087</t>
+  </si>
+  <si>
+    <t>2022-09-20/Normal/1663813938/M03PK5087</t>
+  </si>
+  <si>
+    <t>2022-09-22 09:32:18</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 20/09/2022 pk 5074</t>
+  </si>
+  <si>
+    <t>2022-09-20/Normal/1663814055/M03PK5074</t>
+  </si>
+  <si>
+    <t>2022-09-22 09:34:15</t>
+  </si>
+  <si>
+    <t>pinjaman sektor perdagangan september 2022</t>
+  </si>
+  <si>
+    <t>2022-09-15/1663814285/tjsl</t>
+  </si>
+  <si>
+    <t>2022-09-22 04:38:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aktiva Lancar/Piutang Mitra Binaan/Pinjaman/Sektor Peternakan </t>
+  </si>
+  <si>
+    <t>pinjaman sektor peternakan september 2022</t>
+  </si>
+  <si>
+    <t>2022-09-15/1663814719/tjsl</t>
+  </si>
+  <si>
+    <t>2022-09-22 04:45:19</t>
+  </si>
+  <si>
+    <t>2022-09-22</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 22/09/2022 pk 5091</t>
+  </si>
+  <si>
+    <t>2022-09-22/Normal/1663816731/M03PK5091</t>
+  </si>
+  <si>
+    <t>2022-09-22 10:18:51</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 15/07/2022 pk 5080</t>
+  </si>
+  <si>
+    <t>2022-07-15/Normal/1663905708/M03PK5080</t>
+  </si>
+  <si>
+    <t>2022-09-23 11:01:48</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 30/08/2022 pk 5080</t>
+  </si>
+  <si>
+    <t>2022-08-30/Normal/1663905857/M03PK5080</t>
+  </si>
+  <si>
+    <t>2022-09-23 11:04:17</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 04/07/2022 pk 5098</t>
+  </si>
+  <si>
+    <t>2022-07-04/Normal/1663906865/M03PK5098</t>
+  </si>
+  <si>
+    <t>2022-09-23 11:21:05</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 22/08/2022 pk 5098</t>
+  </si>
+  <si>
+    <t>2022-08-22/Normal/1663906932/M03PK5098</t>
+  </si>
+  <si>
+    <t>2022-09-23 11:22:12</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 30/07/2022 pk 5064</t>
+  </si>
+  <si>
+    <t>Gunawan</t>
+  </si>
+  <si>
+    <t>2022-07-30/Normal/1663907742/M03PK5064</t>
+  </si>
+  <si>
+    <t>2022-09-23 11:35:42</t>
+  </si>
+  <si>
+    <t>2022-08-28</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 28/08/2022 pk 5064</t>
+  </si>
+  <si>
+    <t>2022-08-28/Normal/1663907794/M03PK5064</t>
+  </si>
+  <si>
+    <t>2022-09-23 11:36:34</t>
+  </si>
+  <si>
+    <t>2022-09-25</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 25/09/2022 pk 5121</t>
+  </si>
+  <si>
+    <t>2022-09-25/normal/1664160675/M03PK5121</t>
+  </si>
+  <si>
+    <t>2022-09-26 09:51:15</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok Tgl 22/09/2022 pk 4811</t>
+  </si>
+  <si>
+    <t>2022-09-22/Normal/1664160838/M02PK4811</t>
+  </si>
+  <si>
+    <t>2022-09-26 09:53:58</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 05/08/2022 pk 5124</t>
+  </si>
+  <si>
+    <t>Dida Garnida</t>
+  </si>
+  <si>
+    <t>2022-08-05/normal/1664163382/M03PK5124</t>
+  </si>
+  <si>
+    <t>2022-09-26 10:36:22</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 05/09/2022 pk 5124</t>
+  </si>
+  <si>
+    <t>2022-09-05/normal/1664163442/M03PK5124</t>
+  </si>
+  <si>
+    <t>2022-09-26 10:37:22</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 22/09/2022 pk 5063</t>
+  </si>
+  <si>
+    <t>2022-09-22/Normal/1664163937/M03PK5063</t>
+  </si>
+  <si>
+    <t>2022-09-26 10:45:38</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 22/09/2022 pk 5096</t>
+  </si>
+  <si>
+    <t>2022-09-22/Normal/1664164110/M03PK5096</t>
+  </si>
+  <si>
+    <t>2022-09-26 10:48:30</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 22/09/2022 pk 5108</t>
+  </si>
+  <si>
+    <t>2022-09-22/Normal/1664164328/M01PK5108</t>
+  </si>
+  <si>
+    <t>2022-09-26 10:52:08</t>
+  </si>
+  <si>
+    <t>2022-09-26</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 26/09/2022 pk 4913</t>
+  </si>
+  <si>
+    <t>2022-09-26/Normal/1664333872/M03PK4913</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>2022-09-28 09:57:52</t>
+  </si>
+  <si>
+    <t>2022-09-13</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 13/09/2022 pk 5111</t>
+  </si>
+  <si>
+    <t>2022-09-13/Normal/1664417000/M03PK5111</t>
+  </si>
+  <si>
+    <t>2022-09-29 09:03:20</t>
+  </si>
+  <si>
     <t>2022-09-12</t>
   </si>
   <si>
-    <t>Angsuran Pokok dan Jasa Tgl 12/09/2022 pk 5111</t>
-  </si>
-  <si>
-    <t>2022-09-12/Normal/1663813335/M03PK5111</t>
-  </si>
-  <si>
-    <t>2022-09-22 09:22:15</t>
-  </si>
-  <si>
-    <t>2022-09-14</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 14/09/2022 pk 5097</t>
-  </si>
-  <si>
-    <t>2022-09-14/Normal/1663813479/M02PK5097</t>
-  </si>
-  <si>
-    <t>2022-09-22 09:24:39</t>
-  </si>
-  <si>
-    <t>2022-09-15</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 15/09/2022 pk 5086</t>
-  </si>
-  <si>
-    <t>2022-09-15/Normal/1663813592/M03PK5086</t>
-  </si>
-  <si>
-    <t>2022-09-22 09:26:32</t>
-  </si>
-  <si>
-    <t>2022-09-19</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 19/09/2022 pk 5090</t>
-  </si>
-  <si>
-    <t>2022-09-19/Normal/1663813725/M03PK5090</t>
-  </si>
-  <si>
-    <t>2022-09-22 09:28:45</t>
-  </si>
-  <si>
-    <t>2022-09-20</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 20/09/2022 pk 5087</t>
-  </si>
-  <si>
-    <t>2022-09-20/Normal/1663813938/M03PK5087</t>
-  </si>
-  <si>
-    <t>2022-09-22 09:32:18</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 20/09/2022 pk 5074</t>
-  </si>
-  <si>
-    <t>2022-09-20/Normal/1663814055/M03PK5074</t>
-  </si>
-  <si>
-    <t>2022-09-22 09:34:15</t>
-  </si>
-  <si>
-    <t>pinjaman sektor perdagangan september 2022</t>
-  </si>
-  <si>
-    <t>2022-09-15/1663814285/tjsl</t>
-  </si>
-  <si>
-    <t>2022-09-22 04:38:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aktiva Lancar/Piutang Mitra Binaan/Pinjaman/Sektor Peternakan </t>
-  </si>
-  <si>
-    <t>pinjaman sektor peternakan september 2022</t>
-  </si>
-  <si>
-    <t>2022-09-15/1663814719/tjsl</t>
-  </si>
-  <si>
-    <t>2022-09-22 04:45:19</t>
-  </si>
-  <si>
-    <t>2022-09-22</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 22/09/2022 pk 5091</t>
-  </si>
-  <si>
-    <t>2022-09-22/Normal/1663816731/M03PK5091</t>
-  </si>
-  <si>
-    <t>2022-09-22 10:18:51</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 15/07/2022 pk 5080</t>
-  </si>
-  <si>
-    <t>2022-07-15/Normal/1663905708/M03PK5080</t>
-  </si>
-  <si>
-    <t>2022-09-23 11:01:48</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 30/08/2022 pk 5080</t>
-  </si>
-  <si>
-    <t>2022-08-30/Normal/1663905857/M03PK5080</t>
-  </si>
-  <si>
-    <t>2022-09-23 11:04:17</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 04/07/2022 pk 5098</t>
-  </si>
-  <si>
-    <t>2022-07-04/Normal/1663906865/M03PK5098</t>
-  </si>
-  <si>
-    <t>2022-09-23 11:21:05</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 22/08/2022 pk 5098</t>
-  </si>
-  <si>
-    <t>2022-08-22/Normal/1663906932/M03PK5098</t>
-  </si>
-  <si>
-    <t>2022-09-23 11:22:12</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 30/07/2022 pk 5064</t>
-  </si>
-  <si>
-    <t>Gunawan</t>
-  </si>
-  <si>
-    <t>2022-07-30/Normal/1663907742/M03PK5064</t>
-  </si>
-  <si>
-    <t>2022-09-23 11:35:42</t>
-  </si>
-  <si>
-    <t>2022-08-28</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 28/08/2022 pk 5064</t>
-  </si>
-  <si>
-    <t>2022-08-28/Normal/1663907794/M03PK5064</t>
-  </si>
-  <si>
-    <t>2022-09-23 11:36:34</t>
-  </si>
-  <si>
-    <t>2022-09-25</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 25/09/2022 pk 5121</t>
-  </si>
-  <si>
-    <t>2022-09-25/normal/1664160675/M03PK5121</t>
-  </si>
-  <si>
-    <t>2022-09-26 09:51:15</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok Tgl 22/09/2022 pk 4811</t>
-  </si>
-  <si>
-    <t>2022-09-22/Normal/1664160838/M02PK4811</t>
-  </si>
-  <si>
-    <t>2022-09-26 09:53:58</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 05/08/2022 pk 5124</t>
-  </si>
-  <si>
-    <t>Dida Garnida</t>
-  </si>
-  <si>
-    <t>2022-08-05/normal/1664163382/M03PK5124</t>
-  </si>
-  <si>
-    <t>2022-09-26 10:36:22</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 05/09/2022 pk 5124</t>
-  </si>
-  <si>
-    <t>2022-09-05/normal/1664163442/M03PK5124</t>
-  </si>
-  <si>
-    <t>2022-09-26 10:37:22</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 22/09/2022 pk 5063</t>
-  </si>
-  <si>
-    <t>2022-09-22/Normal/1664163937/M03PK5063</t>
-  </si>
-  <si>
-    <t>2022-09-26 10:45:38</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 22/09/2022 pk 5096</t>
-  </si>
-  <si>
-    <t>2022-09-22/Normal/1664164110/M03PK5096</t>
-  </si>
-  <si>
-    <t>2022-09-26 10:48:30</t>
-  </si>
-  <si>
-    <t>Angsuran Pokok dan Jasa Tgl 22/09/2022 pk 5108</t>
-  </si>
-  <si>
-    <t>2022-09-22/Normal/1664164328/M01PK5108</t>
-  </si>
-  <si>
-    <t>2022-09-26 10:52:08</t>
-  </si>
-  <si>
-    <t>2022-09-26</t>
-  </si>
-  <si>
-    <t>ENJANG CARDA/Angsuran Pokok dan Jasa Tgl 26/09/2022 pk 1798</t>
-  </si>
-  <si>
-    <t>2022-09-26/MASALAH/1664179930/M03PK1798</t>
-  </si>
-  <si>
-    <t>2022-09-26 15:12:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aktiva Lain-lain/Piutang Bermasalah/Angsuran/Sektor Peternakan </t>
+    <t>Angsuran Pokok dan Jasa Tgl 12/09/2022 pk 5073</t>
+  </si>
+  <si>
+    <t>2022-09-12/Normal/1664421673/M03PK5073</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:21:13</t>
+  </si>
+  <si>
+    <t>2022-09-21</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 21/09/2022 pk 5061</t>
+  </si>
+  <si>
+    <t>2022-09-21/Normal/1664421753/M03PK5061</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:22:33</t>
+  </si>
+  <si>
+    <t>2022-09-27</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 27/09/2022 pk 5062</t>
+  </si>
+  <si>
+    <t>2022-09-27/Normal/1664421834/M03PK5062</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:23:54</t>
+  </si>
+  <si>
+    <t>2022-09-28</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 28/09/2022 pk 5077</t>
+  </si>
+  <si>
+    <t>2022-09-28/Normal/1664421921/M03PK5077</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:25:21</t>
+  </si>
+  <si>
+    <t>beban adm dan umum september 2022</t>
+  </si>
+  <si>
+    <t>2022-09-09/1664422666/tjsl</t>
+  </si>
+  <si>
+    <t>2022-09-29 05:37:46</t>
+  </si>
+  <si>
+    <t>beban adm dan umum September 2022</t>
+  </si>
+  <si>
+    <t>2022-09-25/1664422852/tjsl</t>
+  </si>
+  <si>
+    <t>2022-09-29 05:40:52</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 26/09/2022 pk 5103</t>
+  </si>
+  <si>
+    <t>2022-09-26/Normal/1664505051/M03PK5103</t>
+  </si>
+  <si>
+    <t>2022-09-30 09:30:51</t>
+  </si>
+  <si>
+    <t>Pendapatan Jasa Giro september 2022</t>
+  </si>
+  <si>
+    <t>2022-09-25/1664421105/tjsl/tjsl/2022-09-25/1664506012</t>
+  </si>
+  <si>
+    <t>2022-09-30 04:46:52</t>
+  </si>
+  <si>
+    <t>Angsuran Pokok dan Jasa Tgl 31/03/2022 pk 4229</t>
+  </si>
+  <si>
+    <t>2022-03-31/Normal/1664512230/M01PK4229</t>
+  </si>
+  <si>
+    <t>2022-09-30 11:30:30</t>
   </si>
 </sst>
 </file>
@@ -8175,7 +8268,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O2233"/>
+  <dimension ref="A1:O2258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -100676,29 +100769,29 @@
     </row>
     <row r="2168" spans="1:15">
       <c r="A2168">
-        <v>77270</v>
+        <v>77273</v>
       </c>
       <c r="B2168">
-        <v>101010204</v>
+        <v>101010201</v>
       </c>
       <c r="C2168" t="s">
         <v>2526</v>
       </c>
       <c r="D2168">
-        <v>2500000.0</v>
+        <v>4450000.0</v>
       </c>
       <c r="E2168">
         <v>0.0</v>
       </c>
       <c r="F2168">
-        <v>2500000.0</v>
+        <v>4450000.0</v>
       </c>
       <c r="G2168"/>
       <c r="H2168" t="s">
         <v>2527</v>
       </c>
       <c r="I2168" t="s">
-        <v>234</v>
+        <v>90</v>
       </c>
       <c r="J2168" t="s">
         <v>2528</v>
@@ -100718,7 +100811,7 @@
     </row>
     <row r="2169" spans="1:15">
       <c r="A2169">
-        <v>77271</v>
+        <v>77274</v>
       </c>
       <c r="B2169">
         <v>403010100</v>
@@ -100730,7 +100823,7 @@
         <v>0.0</v>
       </c>
       <c r="E2169">
-        <v>250000.0</v>
+        <v>475000.0</v>
       </c>
       <c r="F2169">
         <v>0</v>
@@ -100740,7 +100833,7 @@
         <v>2527</v>
       </c>
       <c r="I2169" t="s">
-        <v>234</v>
+        <v>90</v>
       </c>
       <c r="J2169" t="s">
         <v>2528</v>
@@ -100760,7 +100853,7 @@
     </row>
     <row r="2170" spans="1:15">
       <c r="A2170">
-        <v>77272</v>
+        <v>77275</v>
       </c>
       <c r="B2170">
         <v>101060202</v>
@@ -100772,7 +100865,7 @@
         <v>0.0</v>
       </c>
       <c r="E2170">
-        <v>2250000.0</v>
+        <v>3975000.0</v>
       </c>
       <c r="F2170">
         <v>0</v>
@@ -100784,7 +100877,7 @@
         <v>2527</v>
       </c>
       <c r="I2170" t="s">
-        <v>234</v>
+        <v>90</v>
       </c>
       <c r="J2170" t="s">
         <v>2528</v>
@@ -100804,29 +100897,29 @@
     </row>
     <row r="2171" spans="1:15">
       <c r="A2171">
-        <v>77273</v>
+        <v>77276</v>
       </c>
       <c r="B2171">
-        <v>101010201</v>
+        <v>101010204</v>
       </c>
       <c r="C2171" t="s">
         <v>2530</v>
       </c>
       <c r="D2171">
-        <v>4450000.0</v>
+        <v>2334000.0</v>
       </c>
       <c r="E2171">
         <v>0.0</v>
       </c>
       <c r="F2171">
-        <v>4450000.0</v>
+        <v>2334000.0</v>
       </c>
       <c r="G2171"/>
       <c r="H2171" t="s">
         <v>2531</v>
       </c>
       <c r="I2171" t="s">
-        <v>90</v>
+        <v>242</v>
       </c>
       <c r="J2171" t="s">
         <v>2532</v>
@@ -100846,7 +100939,7 @@
     </row>
     <row r="2172" spans="1:15">
       <c r="A2172">
-        <v>77274</v>
+        <v>77277</v>
       </c>
       <c r="B2172">
         <v>403010100</v>
@@ -100858,7 +100951,7 @@
         <v>0.0</v>
       </c>
       <c r="E2172">
-        <v>475000.0</v>
+        <v>250000.0</v>
       </c>
       <c r="F2172">
         <v>0</v>
@@ -100868,7 +100961,7 @@
         <v>2531</v>
       </c>
       <c r="I2172" t="s">
-        <v>90</v>
+        <v>242</v>
       </c>
       <c r="J2172" t="s">
         <v>2532</v>
@@ -100888,10 +100981,10 @@
     </row>
     <row r="2173" spans="1:15">
       <c r="A2173">
-        <v>77275</v>
+        <v>77278</v>
       </c>
       <c r="B2173">
-        <v>101060202</v>
+        <v>101060201</v>
       </c>
       <c r="C2173" t="s">
         <v>2530</v>
@@ -100900,7 +100993,7 @@
         <v>0.0</v>
       </c>
       <c r="E2173">
-        <v>3975000.0</v>
+        <v>2084000.0</v>
       </c>
       <c r="F2173">
         <v>0</v>
@@ -100912,7 +101005,7 @@
         <v>2531</v>
       </c>
       <c r="I2173" t="s">
-        <v>90</v>
+        <v>242</v>
       </c>
       <c r="J2173" t="s">
         <v>2532</v>
@@ -100932,7 +101025,7 @@
     </row>
     <row r="2174" spans="1:15">
       <c r="A2174">
-        <v>77276</v>
+        <v>77279</v>
       </c>
       <c r="B2174">
         <v>101010204</v>
@@ -100941,20 +101034,20 @@
         <v>2534</v>
       </c>
       <c r="D2174">
-        <v>2334000.0</v>
+        <v>2250000.0</v>
       </c>
       <c r="E2174">
         <v>0.0</v>
       </c>
       <c r="F2174">
-        <v>2334000.0</v>
+        <v>2250000.0</v>
       </c>
       <c r="G2174"/>
       <c r="H2174" t="s">
         <v>2535</v>
       </c>
       <c r="I2174" t="s">
-        <v>242</v>
+        <v>330</v>
       </c>
       <c r="J2174" t="s">
         <v>2536</v>
@@ -100974,7 +101067,7 @@
     </row>
     <row r="2175" spans="1:15">
       <c r="A2175">
-        <v>77277</v>
+        <v>77280</v>
       </c>
       <c r="B2175">
         <v>403010100</v>
@@ -100986,7 +101079,7 @@
         <v>0.0</v>
       </c>
       <c r="E2175">
-        <v>250000.0</v>
+        <v>225000.0</v>
       </c>
       <c r="F2175">
         <v>0</v>
@@ -100996,7 +101089,7 @@
         <v>2535</v>
       </c>
       <c r="I2175" t="s">
-        <v>242</v>
+        <v>330</v>
       </c>
       <c r="J2175" t="s">
         <v>2536</v>
@@ -101016,7 +101109,7 @@
     </row>
     <row r="2176" spans="1:15">
       <c r="A2176">
-        <v>77278</v>
+        <v>77281</v>
       </c>
       <c r="B2176">
         <v>101060201</v>
@@ -101028,7 +101121,7 @@
         <v>0.0</v>
       </c>
       <c r="E2176">
-        <v>2084000.0</v>
+        <v>2025000.0</v>
       </c>
       <c r="F2176">
         <v>0</v>
@@ -101040,7 +101133,7 @@
         <v>2535</v>
       </c>
       <c r="I2176" t="s">
-        <v>242</v>
+        <v>330</v>
       </c>
       <c r="J2176" t="s">
         <v>2536</v>
@@ -101060,7 +101153,7 @@
     </row>
     <row r="2177" spans="1:15">
       <c r="A2177">
-        <v>77279</v>
+        <v>77282</v>
       </c>
       <c r="B2177">
         <v>101010204</v>
@@ -101069,20 +101162,20 @@
         <v>2538</v>
       </c>
       <c r="D2177">
-        <v>2250000.0</v>
+        <v>1400000.0</v>
       </c>
       <c r="E2177">
         <v>0.0</v>
       </c>
       <c r="F2177">
-        <v>2250000.0</v>
+        <v>1400000.0</v>
       </c>
       <c r="G2177"/>
       <c r="H2177" t="s">
         <v>2539</v>
       </c>
       <c r="I2177" t="s">
-        <v>330</v>
+        <v>296</v>
       </c>
       <c r="J2177" t="s">
         <v>2540</v>
@@ -101102,7 +101195,7 @@
     </row>
     <row r="2178" spans="1:15">
       <c r="A2178">
-        <v>77280</v>
+        <v>77283</v>
       </c>
       <c r="B2178">
         <v>403010100</v>
@@ -101114,7 +101207,7 @@
         <v>0.0</v>
       </c>
       <c r="E2178">
-        <v>225000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="F2178">
         <v>0</v>
@@ -101124,7 +101217,7 @@
         <v>2539</v>
       </c>
       <c r="I2178" t="s">
-        <v>330</v>
+        <v>296</v>
       </c>
       <c r="J2178" t="s">
         <v>2540</v>
@@ -101144,10 +101237,10 @@
     </row>
     <row r="2179" spans="1:15">
       <c r="A2179">
-        <v>77281</v>
+        <v>77284</v>
       </c>
       <c r="B2179">
-        <v>101060201</v>
+        <v>101060202</v>
       </c>
       <c r="C2179" t="s">
         <v>2538</v>
@@ -101156,7 +101249,7 @@
         <v>0.0</v>
       </c>
       <c r="E2179">
-        <v>2025000.0</v>
+        <v>1100000.0</v>
       </c>
       <c r="F2179">
         <v>0</v>
@@ -101168,7 +101261,7 @@
         <v>2539</v>
       </c>
       <c r="I2179" t="s">
-        <v>330</v>
+        <v>296</v>
       </c>
       <c r="J2179" t="s">
         <v>2540</v>
@@ -101188,32 +101281,32 @@
     </row>
     <row r="2180" spans="1:15">
       <c r="A2180">
-        <v>77282</v>
+        <v>77285</v>
       </c>
       <c r="B2180">
         <v>101010204</v>
       </c>
       <c r="C2180" t="s">
-        <v>2542</v>
+        <v>2538</v>
       </c>
       <c r="D2180">
-        <v>1400000.0</v>
+        <v>1000000.0</v>
       </c>
       <c r="E2180">
         <v>0.0</v>
       </c>
       <c r="F2180">
-        <v>1400000.0</v>
+        <v>1000000.0</v>
       </c>
       <c r="G2180"/>
       <c r="H2180" t="s">
+        <v>2542</v>
+      </c>
+      <c r="I2180" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2180" t="s">
         <v>2543</v>
-      </c>
-      <c r="I2180" t="s">
-        <v>296</v>
-      </c>
-      <c r="J2180" t="s">
-        <v>2544</v>
       </c>
       <c r="K2180">
         <v>0.0</v>
@@ -101225,37 +101318,37 @@
         <v>2415</v>
       </c>
       <c r="N2180" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="2181" spans="1:15">
       <c r="A2181">
-        <v>77283</v>
+        <v>77286</v>
       </c>
       <c r="B2181">
         <v>403010100</v>
       </c>
       <c r="C2181" t="s">
-        <v>2542</v>
+        <v>2538</v>
       </c>
       <c r="D2181">
         <v>0.0</v>
       </c>
       <c r="E2181">
-        <v>300000.0</v>
+        <v>250000.0</v>
       </c>
       <c r="F2181">
         <v>0</v>
       </c>
       <c r="G2181"/>
       <c r="H2181" t="s">
+        <v>2542</v>
+      </c>
+      <c r="I2181" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2181" t="s">
         <v>2543</v>
-      </c>
-      <c r="I2181" t="s">
-        <v>296</v>
-      </c>
-      <c r="J2181" t="s">
-        <v>2544</v>
       </c>
       <c r="K2181">
         <v>0.0</v>
@@ -101267,24 +101360,24 @@
         <v>2415</v>
       </c>
       <c r="N2181" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="2182" spans="1:15">
       <c r="A2182">
-        <v>77284</v>
+        <v>77287</v>
       </c>
       <c r="B2182">
         <v>101060202</v>
       </c>
       <c r="C2182" t="s">
-        <v>2542</v>
+        <v>2538</v>
       </c>
       <c r="D2182">
         <v>0.0</v>
       </c>
       <c r="E2182">
-        <v>1100000.0</v>
+        <v>750000.0</v>
       </c>
       <c r="F2182">
         <v>0</v>
@@ -101293,13 +101386,13 @@
         <v>15</v>
       </c>
       <c r="H2182" t="s">
+        <v>2542</v>
+      </c>
+      <c r="I2182" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2182" t="s">
         <v>2543</v>
-      </c>
-      <c r="I2182" t="s">
-        <v>296</v>
-      </c>
-      <c r="J2182" t="s">
-        <v>2544</v>
       </c>
       <c r="K2182">
         <v>0.0</v>
@@ -101311,37 +101404,37 @@
         <v>2415</v>
       </c>
       <c r="N2182" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="2183" spans="1:15">
       <c r="A2183">
-        <v>77285</v>
+        <v>77288</v>
       </c>
       <c r="B2183">
-        <v>101010204</v>
+        <v>101060102</v>
       </c>
       <c r="C2183" t="s">
-        <v>2542</v>
+        <v>2530</v>
       </c>
       <c r="D2183">
-        <v>1000000.0</v>
+        <v>290000000.0</v>
       </c>
       <c r="E2183">
         <v>0.0</v>
       </c>
       <c r="F2183">
-        <v>1000000.0</v>
+        <v>290000000.0</v>
       </c>
       <c r="G2183"/>
       <c r="H2183" t="s">
+        <v>696</v>
+      </c>
+      <c r="I2183" t="s">
+        <v>2545</v>
+      </c>
+      <c r="J2183" t="s">
         <v>2546</v>
-      </c>
-      <c r="I2183" t="s">
-        <v>155</v>
-      </c>
-      <c r="J2183" t="s">
-        <v>2547</v>
       </c>
       <c r="K2183">
         <v>0.0</v>
@@ -101353,37 +101446,39 @@
         <v>2415</v>
       </c>
       <c r="N2183" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="2184" spans="1:15">
       <c r="A2184">
-        <v>77286</v>
+        <v>77289</v>
       </c>
       <c r="B2184">
-        <v>403010100</v>
+        <v>101010204</v>
       </c>
       <c r="C2184" t="s">
-        <v>2542</v>
+        <v>2530</v>
       </c>
       <c r="D2184">
         <v>0.0</v>
       </c>
       <c r="E2184">
-        <v>250000.0</v>
+        <v>290000000.0</v>
       </c>
       <c r="F2184">
         <v>0</v>
       </c>
-      <c r="G2184"/>
+      <c r="G2184" t="s">
+        <v>15</v>
+      </c>
       <c r="H2184" t="s">
+        <v>407</v>
+      </c>
+      <c r="I2184" t="s">
+        <v>2545</v>
+      </c>
+      <c r="J2184" t="s">
         <v>2546</v>
-      </c>
-      <c r="I2184" t="s">
-        <v>155</v>
-      </c>
-      <c r="J2184" t="s">
-        <v>2547</v>
       </c>
       <c r="K2184">
         <v>0.0</v>
@@ -101395,39 +101490,37 @@
         <v>2415</v>
       </c>
       <c r="N2184" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="2185" spans="1:15">
       <c r="A2185">
-        <v>77287</v>
+        <v>77290</v>
       </c>
       <c r="B2185">
-        <v>101060202</v>
+        <v>101060106</v>
       </c>
       <c r="C2185" t="s">
-        <v>2542</v>
+        <v>2530</v>
       </c>
       <c r="D2185">
-        <v>0.0</v>
+        <v>20000000.0</v>
       </c>
       <c r="E2185">
-        <v>750000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F2185">
-        <v>0</v>
-      </c>
-      <c r="G2185" t="s">
-        <v>15</v>
-      </c>
+        <v>20000000.0</v>
+      </c>
+      <c r="G2185"/>
       <c r="H2185" t="s">
-        <v>2546</v>
+        <v>2548</v>
       </c>
       <c r="I2185" t="s">
-        <v>155</v>
+        <v>2549</v>
       </c>
       <c r="J2185" t="s">
-        <v>2547</v>
+        <v>2550</v>
       </c>
       <c r="K2185">
         <v>0.0</v>
@@ -101439,31 +101532,33 @@
         <v>2415</v>
       </c>
       <c r="N2185" t="s">
-        <v>2548</v>
+        <v>2551</v>
       </c>
     </row>
     <row r="2186" spans="1:15">
       <c r="A2186">
-        <v>77288</v>
+        <v>77291</v>
       </c>
       <c r="B2186">
-        <v>101060102</v>
+        <v>101010204</v>
       </c>
       <c r="C2186" t="s">
-        <v>2534</v>
+        <v>2530</v>
       </c>
       <c r="D2186">
-        <v>290000000.0</v>
+        <v>0.0</v>
       </c>
       <c r="E2186">
-        <v>0.0</v>
+        <v>20000000.0</v>
       </c>
       <c r="F2186">
-        <v>290000000.0</v>
-      </c>
-      <c r="G2186"/>
+        <v>0</v>
+      </c>
+      <c r="G2186" t="s">
+        <v>15</v>
+      </c>
       <c r="H2186" t="s">
-        <v>696</v>
+        <v>407</v>
       </c>
       <c r="I2186" t="s">
         <v>2549</v>
@@ -101486,34 +101581,32 @@
     </row>
     <row r="2187" spans="1:15">
       <c r="A2187">
-        <v>77289</v>
+        <v>77292</v>
       </c>
       <c r="B2187">
         <v>101010204</v>
       </c>
       <c r="C2187" t="s">
-        <v>2534</v>
+        <v>2552</v>
       </c>
       <c r="D2187">
-        <v>0.0</v>
+        <v>1200000.0</v>
       </c>
       <c r="E2187">
-        <v>290000000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F2187">
-        <v>0</v>
-      </c>
-      <c r="G2187" t="s">
-        <v>15</v>
-      </c>
+        <v>1200000.0</v>
+      </c>
+      <c r="G2187"/>
       <c r="H2187" t="s">
-        <v>407</v>
+        <v>2553</v>
       </c>
       <c r="I2187" t="s">
-        <v>2549</v>
+        <v>230</v>
       </c>
       <c r="J2187" t="s">
-        <v>2550</v>
+        <v>2554</v>
       </c>
       <c r="K2187">
         <v>0.0</v>
@@ -101525,34 +101618,34 @@
         <v>2415</v>
       </c>
       <c r="N2187" t="s">
-        <v>2551</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="2188" spans="1:15">
       <c r="A2188">
-        <v>77290</v>
+        <v>77293</v>
       </c>
       <c r="B2188">
-        <v>101060106</v>
+        <v>403010100</v>
       </c>
       <c r="C2188" t="s">
-        <v>2534</v>
+        <v>2552</v>
       </c>
       <c r="D2188">
-        <v>20000000.0</v>
+        <v>0.0</v>
       </c>
       <c r="E2188">
-        <v>0.0</v>
+        <v>200000.0</v>
       </c>
       <c r="F2188">
-        <v>20000000.0</v>
+        <v>0</v>
       </c>
       <c r="G2188"/>
       <c r="H2188" t="s">
-        <v>2552</v>
+        <v>2553</v>
       </c>
       <c r="I2188" t="s">
-        <v>2553</v>
+        <v>230</v>
       </c>
       <c r="J2188" t="s">
         <v>2554</v>
@@ -101572,19 +101665,19 @@
     </row>
     <row r="2189" spans="1:15">
       <c r="A2189">
-        <v>77291</v>
+        <v>77294</v>
       </c>
       <c r="B2189">
-        <v>101010204</v>
+        <v>101060207</v>
       </c>
       <c r="C2189" t="s">
-        <v>2534</v>
+        <v>2552</v>
       </c>
       <c r="D2189">
         <v>0.0</v>
       </c>
       <c r="E2189">
-        <v>20000000.0</v>
+        <v>1000000.0</v>
       </c>
       <c r="F2189">
         <v>0</v>
@@ -101593,10 +101686,10 @@
         <v>15</v>
       </c>
       <c r="H2189" t="s">
-        <v>407</v>
+        <v>2553</v>
       </c>
       <c r="I2189" t="s">
-        <v>2553</v>
+        <v>230</v>
       </c>
       <c r="J2189" t="s">
         <v>2554</v>
@@ -101616,32 +101709,32 @@
     </row>
     <row r="2190" spans="1:15">
       <c r="A2190">
-        <v>77292</v>
+        <v>77304</v>
       </c>
       <c r="B2190">
         <v>101010204</v>
       </c>
       <c r="C2190" t="s">
-        <v>2556</v>
+        <v>1961</v>
       </c>
       <c r="D2190">
-        <v>1200000.0</v>
+        <v>3500000.0</v>
       </c>
       <c r="E2190">
         <v>0.0</v>
       </c>
       <c r="F2190">
-        <v>1200000.0</v>
+        <v>3500000.0</v>
       </c>
       <c r="G2190"/>
       <c r="H2190" t="s">
+        <v>2556</v>
+      </c>
+      <c r="I2190" t="s">
+        <v>264</v>
+      </c>
+      <c r="J2190" t="s">
         <v>2557</v>
-      </c>
-      <c r="I2190" t="s">
-        <v>230</v>
-      </c>
-      <c r="J2190" t="s">
-        <v>2558</v>
       </c>
       <c r="K2190">
         <v>0.0</v>
@@ -101653,37 +101746,37 @@
         <v>2415</v>
       </c>
       <c r="N2190" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="2191" spans="1:15">
       <c r="A2191">
-        <v>77293</v>
+        <v>77305</v>
       </c>
       <c r="B2191">
         <v>403010100</v>
       </c>
       <c r="C2191" t="s">
-        <v>2556</v>
+        <v>1961</v>
       </c>
       <c r="D2191">
         <v>0.0</v>
       </c>
       <c r="E2191">
-        <v>200000.0</v>
+        <v>375000.0</v>
       </c>
       <c r="F2191">
         <v>0</v>
       </c>
       <c r="G2191"/>
       <c r="H2191" t="s">
+        <v>2556</v>
+      </c>
+      <c r="I2191" t="s">
+        <v>264</v>
+      </c>
+      <c r="J2191" t="s">
         <v>2557</v>
-      </c>
-      <c r="I2191" t="s">
-        <v>230</v>
-      </c>
-      <c r="J2191" t="s">
-        <v>2558</v>
       </c>
       <c r="K2191">
         <v>0.0</v>
@@ -101695,24 +101788,24 @@
         <v>2415</v>
       </c>
       <c r="N2191" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="2192" spans="1:15">
       <c r="A2192">
-        <v>77294</v>
+        <v>77306</v>
       </c>
       <c r="B2192">
-        <v>101060207</v>
+        <v>101060205</v>
       </c>
       <c r="C2192" t="s">
-        <v>2556</v>
+        <v>1961</v>
       </c>
       <c r="D2192">
         <v>0.0</v>
       </c>
       <c r="E2192">
-        <v>1000000.0</v>
+        <v>3125000.0</v>
       </c>
       <c r="F2192">
         <v>0</v>
@@ -101721,13 +101814,13 @@
         <v>15</v>
       </c>
       <c r="H2192" t="s">
+        <v>2556</v>
+      </c>
+      <c r="I2192" t="s">
+        <v>264</v>
+      </c>
+      <c r="J2192" t="s">
         <v>2557</v>
-      </c>
-      <c r="I2192" t="s">
-        <v>230</v>
-      </c>
-      <c r="J2192" t="s">
-        <v>2558</v>
       </c>
       <c r="K2192">
         <v>0.0</v>
@@ -101739,18 +101832,18 @@
         <v>2415</v>
       </c>
       <c r="N2192" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="2193" spans="1:15">
       <c r="A2193">
-        <v>77304</v>
+        <v>77307</v>
       </c>
       <c r="B2193">
         <v>101010204</v>
       </c>
       <c r="C2193" t="s">
-        <v>1961</v>
+        <v>2319</v>
       </c>
       <c r="D2193">
         <v>3500000.0</v>
@@ -101763,13 +101856,13 @@
       </c>
       <c r="G2193"/>
       <c r="H2193" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="I2193" t="s">
         <v>264</v>
       </c>
       <c r="J2193" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="K2193">
         <v>0.0</v>
@@ -101781,18 +101874,18 @@
         <v>2415</v>
       </c>
       <c r="N2193" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="2194" spans="1:15">
       <c r="A2194">
-        <v>77305</v>
+        <v>77308</v>
       </c>
       <c r="B2194">
         <v>403010100</v>
       </c>
       <c r="C2194" t="s">
-        <v>1961</v>
+        <v>2319</v>
       </c>
       <c r="D2194">
         <v>0.0</v>
@@ -101805,13 +101898,13 @@
       </c>
       <c r="G2194"/>
       <c r="H2194" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="I2194" t="s">
         <v>264</v>
       </c>
       <c r="J2194" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="K2194">
         <v>0.0</v>
@@ -101823,18 +101916,18 @@
         <v>2415</v>
       </c>
       <c r="N2194" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="2195" spans="1:15">
       <c r="A2195">
-        <v>77306</v>
+        <v>77309</v>
       </c>
       <c r="B2195">
         <v>101060205</v>
       </c>
       <c r="C2195" t="s">
-        <v>1961</v>
+        <v>2319</v>
       </c>
       <c r="D2195">
         <v>0.0</v>
@@ -101849,13 +101942,13 @@
         <v>15</v>
       </c>
       <c r="H2195" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="I2195" t="s">
         <v>264</v>
       </c>
       <c r="J2195" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="K2195">
         <v>0.0</v>
@@ -101867,37 +101960,37 @@
         <v>2415</v>
       </c>
       <c r="N2195" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="2196" spans="1:15">
       <c r="A2196">
-        <v>77307</v>
+        <v>77310</v>
       </c>
       <c r="B2196">
         <v>101010204</v>
       </c>
       <c r="C2196" t="s">
-        <v>2319</v>
+        <v>1839</v>
       </c>
       <c r="D2196">
-        <v>3500000.0</v>
+        <v>934000.0</v>
       </c>
       <c r="E2196">
         <v>0.0</v>
       </c>
       <c r="F2196">
-        <v>3500000.0</v>
+        <v>934000.0</v>
       </c>
       <c r="G2196"/>
       <c r="H2196" t="s">
+        <v>2562</v>
+      </c>
+      <c r="I2196" t="s">
+        <v>574</v>
+      </c>
+      <c r="J2196" t="s">
         <v>2563</v>
-      </c>
-      <c r="I2196" t="s">
-        <v>264</v>
-      </c>
-      <c r="J2196" t="s">
-        <v>2564</v>
       </c>
       <c r="K2196">
         <v>0.0</v>
@@ -101909,37 +102002,37 @@
         <v>2415</v>
       </c>
       <c r="N2196" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="2197" spans="1:15">
       <c r="A2197">
-        <v>77308</v>
+        <v>77311</v>
       </c>
       <c r="B2197">
         <v>403010100</v>
       </c>
       <c r="C2197" t="s">
-        <v>2319</v>
+        <v>1839</v>
       </c>
       <c r="D2197">
         <v>0.0</v>
       </c>
       <c r="E2197">
-        <v>375000.0</v>
+        <v>200000.0</v>
       </c>
       <c r="F2197">
         <v>0</v>
       </c>
       <c r="G2197"/>
       <c r="H2197" t="s">
+        <v>2562</v>
+      </c>
+      <c r="I2197" t="s">
+        <v>574</v>
+      </c>
+      <c r="J2197" t="s">
         <v>2563</v>
-      </c>
-      <c r="I2197" t="s">
-        <v>264</v>
-      </c>
-      <c r="J2197" t="s">
-        <v>2564</v>
       </c>
       <c r="K2197">
         <v>0.0</v>
@@ -101951,24 +102044,24 @@
         <v>2415</v>
       </c>
       <c r="N2197" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="2198" spans="1:15">
       <c r="A2198">
-        <v>77309</v>
+        <v>77312</v>
       </c>
       <c r="B2198">
-        <v>101060205</v>
+        <v>101060207</v>
       </c>
       <c r="C2198" t="s">
-        <v>2319</v>
+        <v>1839</v>
       </c>
       <c r="D2198">
         <v>0.0</v>
       </c>
       <c r="E2198">
-        <v>3125000.0</v>
+        <v>734000.0</v>
       </c>
       <c r="F2198">
         <v>0</v>
@@ -101977,13 +102070,13 @@
         <v>15</v>
       </c>
       <c r="H2198" t="s">
+        <v>2562</v>
+      </c>
+      <c r="I2198" t="s">
+        <v>574</v>
+      </c>
+      <c r="J2198" t="s">
         <v>2563</v>
-      </c>
-      <c r="I2198" t="s">
-        <v>264</v>
-      </c>
-      <c r="J2198" t="s">
-        <v>2564</v>
       </c>
       <c r="K2198">
         <v>0.0</v>
@@ -101995,18 +102088,18 @@
         <v>2415</v>
       </c>
       <c r="N2198" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="2199" spans="1:15">
       <c r="A2199">
-        <v>77310</v>
+        <v>77313</v>
       </c>
       <c r="B2199">
         <v>101010204</v>
       </c>
       <c r="C2199" t="s">
-        <v>1839</v>
+        <v>2255</v>
       </c>
       <c r="D2199">
         <v>934000.0</v>
@@ -102019,13 +102112,13 @@
       </c>
       <c r="G2199"/>
       <c r="H2199" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="I2199" t="s">
         <v>574</v>
       </c>
       <c r="J2199" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="K2199">
         <v>0.0</v>
@@ -102037,37 +102130,37 @@
         <v>2415</v>
       </c>
       <c r="N2199" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
     </row>
     <row r="2200" spans="1:15">
       <c r="A2200">
-        <v>77311</v>
+        <v>77314</v>
       </c>
       <c r="B2200">
         <v>403010100</v>
       </c>
       <c r="C2200" t="s">
-        <v>1839</v>
+        <v>2255</v>
       </c>
       <c r="D2200">
         <v>0.0</v>
       </c>
       <c r="E2200">
-        <v>200000.0</v>
+        <v>100000.0</v>
       </c>
       <c r="F2200">
         <v>0</v>
       </c>
       <c r="G2200"/>
       <c r="H2200" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="I2200" t="s">
         <v>574</v>
       </c>
       <c r="J2200" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="K2200">
         <v>0.0</v>
@@ -102079,24 +102172,24 @@
         <v>2415</v>
       </c>
       <c r="N2200" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
     </row>
     <row r="2201" spans="1:15">
       <c r="A2201">
-        <v>77312</v>
+        <v>77315</v>
       </c>
       <c r="B2201">
         <v>101060207</v>
       </c>
       <c r="C2201" t="s">
-        <v>1839</v>
+        <v>2255</v>
       </c>
       <c r="D2201">
         <v>0.0</v>
       </c>
       <c r="E2201">
-        <v>734000.0</v>
+        <v>834000.0</v>
       </c>
       <c r="F2201">
         <v>0</v>
@@ -102105,13 +102198,13 @@
         <v>15</v>
       </c>
       <c r="H2201" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="I2201" t="s">
         <v>574</v>
       </c>
       <c r="J2201" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="K2201">
         <v>0.0</v>
@@ -102123,34 +102216,34 @@
         <v>2415</v>
       </c>
       <c r="N2201" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
     </row>
     <row r="2202" spans="1:15">
       <c r="A2202">
-        <v>77313</v>
+        <v>77316</v>
       </c>
       <c r="B2202">
         <v>101010204</v>
       </c>
       <c r="C2202" t="s">
-        <v>2255</v>
+        <v>2011</v>
       </c>
       <c r="D2202">
-        <v>934000.0</v>
+        <v>1350000.0</v>
       </c>
       <c r="E2202">
         <v>0.0</v>
       </c>
       <c r="F2202">
-        <v>934000.0</v>
+        <v>1350000.0</v>
       </c>
       <c r="G2202"/>
       <c r="H2202" t="s">
+        <v>2568</v>
+      </c>
+      <c r="I2202" t="s">
         <v>2569</v>
-      </c>
-      <c r="I2202" t="s">
-        <v>574</v>
       </c>
       <c r="J2202" t="s">
         <v>2570</v>
@@ -102170,29 +102263,29 @@
     </row>
     <row r="2203" spans="1:15">
       <c r="A2203">
-        <v>77314</v>
+        <v>77317</v>
       </c>
       <c r="B2203">
         <v>403010100</v>
       </c>
       <c r="C2203" t="s">
-        <v>2255</v>
+        <v>2011</v>
       </c>
       <c r="D2203">
         <v>0.0</v>
       </c>
       <c r="E2203">
-        <v>100000.0</v>
+        <v>150000.0</v>
       </c>
       <c r="F2203">
         <v>0</v>
       </c>
       <c r="G2203"/>
       <c r="H2203" t="s">
+        <v>2568</v>
+      </c>
+      <c r="I2203" t="s">
         <v>2569</v>
-      </c>
-      <c r="I2203" t="s">
-        <v>574</v>
       </c>
       <c r="J2203" t="s">
         <v>2570</v>
@@ -102212,19 +102305,19 @@
     </row>
     <row r="2204" spans="1:15">
       <c r="A2204">
-        <v>77315</v>
+        <v>77318</v>
       </c>
       <c r="B2204">
-        <v>101060207</v>
+        <v>101060202</v>
       </c>
       <c r="C2204" t="s">
-        <v>2255</v>
+        <v>2011</v>
       </c>
       <c r="D2204">
         <v>0.0</v>
       </c>
       <c r="E2204">
-        <v>834000.0</v>
+        <v>1200000.0</v>
       </c>
       <c r="F2204">
         <v>0</v>
@@ -102233,10 +102326,10 @@
         <v>15</v>
       </c>
       <c r="H2204" t="s">
+        <v>2568</v>
+      </c>
+      <c r="I2204" t="s">
         <v>2569</v>
-      </c>
-      <c r="I2204" t="s">
-        <v>574</v>
       </c>
       <c r="J2204" t="s">
         <v>2570</v>
@@ -102256,29 +102349,29 @@
     </row>
     <row r="2205" spans="1:15">
       <c r="A2205">
-        <v>77316</v>
+        <v>77319</v>
       </c>
       <c r="B2205">
         <v>101010204</v>
       </c>
       <c r="C2205" t="s">
-        <v>2011</v>
+        <v>2572</v>
       </c>
       <c r="D2205">
-        <v>1350000.0</v>
+        <v>2650000.0</v>
       </c>
       <c r="E2205">
         <v>0.0</v>
       </c>
       <c r="F2205">
-        <v>1350000.0</v>
+        <v>2650000.0</v>
       </c>
       <c r="G2205"/>
       <c r="H2205" t="s">
-        <v>2572</v>
+        <v>2573</v>
       </c>
       <c r="I2205" t="s">
-        <v>2573</v>
+        <v>2569</v>
       </c>
       <c r="J2205" t="s">
         <v>2574</v>
@@ -102298,13 +102391,13 @@
     </row>
     <row r="2206" spans="1:15">
       <c r="A2206">
-        <v>77317</v>
+        <v>77320</v>
       </c>
       <c r="B2206">
         <v>403010100</v>
       </c>
       <c r="C2206" t="s">
-        <v>2011</v>
+        <v>2572</v>
       </c>
       <c r="D2206">
         <v>0.0</v>
@@ -102317,10 +102410,10 @@
       </c>
       <c r="G2206"/>
       <c r="H2206" t="s">
-        <v>2572</v>
+        <v>2573</v>
       </c>
       <c r="I2206" t="s">
-        <v>2573</v>
+        <v>2569</v>
       </c>
       <c r="J2206" t="s">
         <v>2574</v>
@@ -102340,19 +102433,19 @@
     </row>
     <row r="2207" spans="1:15">
       <c r="A2207">
-        <v>77318</v>
+        <v>77321</v>
       </c>
       <c r="B2207">
         <v>101060202</v>
       </c>
       <c r="C2207" t="s">
-        <v>2011</v>
+        <v>2572</v>
       </c>
       <c r="D2207">
         <v>0.0</v>
       </c>
       <c r="E2207">
-        <v>1200000.0</v>
+        <v>2500000.0</v>
       </c>
       <c r="F2207">
         <v>0</v>
@@ -102361,10 +102454,10 @@
         <v>15</v>
       </c>
       <c r="H2207" t="s">
-        <v>2572</v>
+        <v>2573</v>
       </c>
       <c r="I2207" t="s">
-        <v>2573</v>
+        <v>2569</v>
       </c>
       <c r="J2207" t="s">
         <v>2574</v>
@@ -102384,7 +102477,7 @@
     </row>
     <row r="2208" spans="1:15">
       <c r="A2208">
-        <v>77319</v>
+        <v>77342</v>
       </c>
       <c r="B2208">
         <v>101010204</v>
@@ -102393,20 +102486,20 @@
         <v>2576</v>
       </c>
       <c r="D2208">
-        <v>2650000.0</v>
+        <v>1900000.0</v>
       </c>
       <c r="E2208">
         <v>0.0</v>
       </c>
       <c r="F2208">
-        <v>2650000.0</v>
+        <v>1900000.0</v>
       </c>
       <c r="G2208"/>
       <c r="H2208" t="s">
         <v>2577</v>
       </c>
       <c r="I2208" t="s">
-        <v>2573</v>
+        <v>2271</v>
       </c>
       <c r="J2208" t="s">
         <v>2578</v>
@@ -102426,7 +102519,7 @@
     </row>
     <row r="2209" spans="1:15">
       <c r="A2209">
-        <v>77320</v>
+        <v>77343</v>
       </c>
       <c r="B2209">
         <v>403010100</v>
@@ -102438,7 +102531,7 @@
         <v>0.0</v>
       </c>
       <c r="E2209">
-        <v>150000.0</v>
+        <v>200000.0</v>
       </c>
       <c r="F2209">
         <v>0</v>
@@ -102448,7 +102541,7 @@
         <v>2577</v>
       </c>
       <c r="I2209" t="s">
-        <v>2573</v>
+        <v>2271</v>
       </c>
       <c r="J2209" t="s">
         <v>2578</v>
@@ -102468,10 +102561,10 @@
     </row>
     <row r="2210" spans="1:15">
       <c r="A2210">
-        <v>77321</v>
+        <v>77344</v>
       </c>
       <c r="B2210">
-        <v>101060202</v>
+        <v>101060201</v>
       </c>
       <c r="C2210" t="s">
         <v>2576</v>
@@ -102480,7 +102573,7 @@
         <v>0.0</v>
       </c>
       <c r="E2210">
-        <v>2500000.0</v>
+        <v>1700000.0</v>
       </c>
       <c r="F2210">
         <v>0</v>
@@ -102492,7 +102585,7 @@
         <v>2577</v>
       </c>
       <c r="I2210" t="s">
-        <v>2573</v>
+        <v>2271</v>
       </c>
       <c r="J2210" t="s">
         <v>2578</v>
@@ -102512,32 +102605,32 @@
     </row>
     <row r="2211" spans="1:15">
       <c r="A2211">
-        <v>77342</v>
+        <v>77345</v>
       </c>
       <c r="B2211">
-        <v>101010204</v>
+        <v>101010201</v>
       </c>
       <c r="C2211" t="s">
-        <v>2580</v>
+        <v>2552</v>
       </c>
       <c r="D2211">
-        <v>1900000.0</v>
+        <v>500000.0</v>
       </c>
       <c r="E2211">
         <v>0.0</v>
       </c>
       <c r="F2211">
-        <v>1900000.0</v>
+        <v>500000.0</v>
       </c>
       <c r="G2211"/>
       <c r="H2211" t="s">
+        <v>2580</v>
+      </c>
+      <c r="I2211" t="s">
+        <v>1946</v>
+      </c>
+      <c r="J2211" t="s">
         <v>2581</v>
-      </c>
-      <c r="I2211" t="s">
-        <v>2271</v>
-      </c>
-      <c r="J2211" t="s">
-        <v>2582</v>
       </c>
       <c r="K2211">
         <v>0.0</v>
@@ -102549,37 +102642,37 @@
         <v>2415</v>
       </c>
       <c r="N2211" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="2212" spans="1:15">
       <c r="A2212">
-        <v>77343</v>
+        <v>77346</v>
       </c>
       <c r="B2212">
         <v>403010100</v>
       </c>
       <c r="C2212" t="s">
-        <v>2580</v>
+        <v>2552</v>
       </c>
       <c r="D2212">
         <v>0.0</v>
       </c>
       <c r="E2212">
-        <v>200000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F2212">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G2212"/>
       <c r="H2212" t="s">
+        <v>2580</v>
+      </c>
+      <c r="I2212" t="s">
+        <v>1946</v>
+      </c>
+      <c r="J2212" t="s">
         <v>2581</v>
-      </c>
-      <c r="I2212" t="s">
-        <v>2271</v>
-      </c>
-      <c r="J2212" t="s">
-        <v>2582</v>
       </c>
       <c r="K2212">
         <v>0.0</v>
@@ -102591,24 +102684,24 @@
         <v>2415</v>
       </c>
       <c r="N2212" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="2213" spans="1:15">
       <c r="A2213">
-        <v>77344</v>
+        <v>77347</v>
       </c>
       <c r="B2213">
-        <v>101060201</v>
+        <v>101060202</v>
       </c>
       <c r="C2213" t="s">
-        <v>2580</v>
+        <v>2552</v>
       </c>
       <c r="D2213">
         <v>0.0</v>
       </c>
       <c r="E2213">
-        <v>1700000.0</v>
+        <v>500000.0</v>
       </c>
       <c r="F2213">
         <v>0</v>
@@ -102617,13 +102710,13 @@
         <v>15</v>
       </c>
       <c r="H2213" t="s">
+        <v>2580</v>
+      </c>
+      <c r="I2213" t="s">
+        <v>1946</v>
+      </c>
+      <c r="J2213" t="s">
         <v>2581</v>
-      </c>
-      <c r="I2213" t="s">
-        <v>2271</v>
-      </c>
-      <c r="J2213" t="s">
-        <v>2582</v>
       </c>
       <c r="K2213">
         <v>0.0</v>
@@ -102635,34 +102728,34 @@
         <v>2415</v>
       </c>
       <c r="N2213" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="2214" spans="1:15">
       <c r="A2214">
-        <v>77345</v>
+        <v>77348</v>
       </c>
       <c r="B2214">
-        <v>101010201</v>
+        <v>101010204</v>
       </c>
       <c r="C2214" t="s">
-        <v>2556</v>
+        <v>2179</v>
       </c>
       <c r="D2214">
-        <v>500000.0</v>
+        <v>2334000.0</v>
       </c>
       <c r="E2214">
         <v>0.0</v>
       </c>
       <c r="F2214">
-        <v>500000.0</v>
+        <v>2334000.0</v>
       </c>
       <c r="G2214"/>
       <c r="H2214" t="s">
+        <v>2583</v>
+      </c>
+      <c r="I2214" t="s">
         <v>2584</v>
-      </c>
-      <c r="I2214" t="s">
-        <v>1946</v>
       </c>
       <c r="J2214" t="s">
         <v>2585</v>
@@ -102682,29 +102775,29 @@
     </row>
     <row r="2215" spans="1:15">
       <c r="A2215">
-        <v>77346</v>
+        <v>77349</v>
       </c>
       <c r="B2215">
         <v>403010100</v>
       </c>
       <c r="C2215" t="s">
-        <v>2556</v>
+        <v>2179</v>
       </c>
       <c r="D2215">
         <v>0.0</v>
       </c>
       <c r="E2215">
-        <v>0.0</v>
+        <v>250000.0</v>
       </c>
       <c r="F2215">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G2215"/>
       <c r="H2215" t="s">
+        <v>2583</v>
+      </c>
+      <c r="I2215" t="s">
         <v>2584</v>
-      </c>
-      <c r="I2215" t="s">
-        <v>1946</v>
       </c>
       <c r="J2215" t="s">
         <v>2585</v>
@@ -102724,19 +102817,19 @@
     </row>
     <row r="2216" spans="1:15">
       <c r="A2216">
-        <v>77347</v>
+        <v>77350</v>
       </c>
       <c r="B2216">
-        <v>101060202</v>
+        <v>101060207</v>
       </c>
       <c r="C2216" t="s">
-        <v>2556</v>
+        <v>2179</v>
       </c>
       <c r="D2216">
         <v>0.0</v>
       </c>
       <c r="E2216">
-        <v>500000.0</v>
+        <v>2084000.0</v>
       </c>
       <c r="F2216">
         <v>0</v>
@@ -102745,10 +102838,10 @@
         <v>15</v>
       </c>
       <c r="H2216" t="s">
+        <v>2583</v>
+      </c>
+      <c r="I2216" t="s">
         <v>2584</v>
-      </c>
-      <c r="I2216" t="s">
-        <v>1946</v>
       </c>
       <c r="J2216" t="s">
         <v>2585</v>
@@ -102768,13 +102861,13 @@
     </row>
     <row r="2217" spans="1:15">
       <c r="A2217">
-        <v>77348</v>
+        <v>77351</v>
       </c>
       <c r="B2217">
         <v>101010204</v>
       </c>
       <c r="C2217" t="s">
-        <v>2179</v>
+        <v>2445</v>
       </c>
       <c r="D2217">
         <v>2334000.0</v>
@@ -102790,10 +102883,10 @@
         <v>2587</v>
       </c>
       <c r="I2217" t="s">
+        <v>2584</v>
+      </c>
+      <c r="J2217" t="s">
         <v>2588</v>
-      </c>
-      <c r="J2217" t="s">
-        <v>2589</v>
       </c>
       <c r="K2217">
         <v>0.0</v>
@@ -102805,18 +102898,18 @@
         <v>2415</v>
       </c>
       <c r="N2217" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="2218" spans="1:15">
       <c r="A2218">
-        <v>77349</v>
+        <v>77352</v>
       </c>
       <c r="B2218">
         <v>403010100</v>
       </c>
       <c r="C2218" t="s">
-        <v>2179</v>
+        <v>2445</v>
       </c>
       <c r="D2218">
         <v>0.0</v>
@@ -102832,10 +102925,10 @@
         <v>2587</v>
       </c>
       <c r="I2218" t="s">
+        <v>2584</v>
+      </c>
+      <c r="J2218" t="s">
         <v>2588</v>
-      </c>
-      <c r="J2218" t="s">
-        <v>2589</v>
       </c>
       <c r="K2218">
         <v>0.0</v>
@@ -102847,18 +102940,18 @@
         <v>2415</v>
       </c>
       <c r="N2218" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="2219" spans="1:15">
       <c r="A2219">
-        <v>77350</v>
+        <v>77353</v>
       </c>
       <c r="B2219">
         <v>101060207</v>
       </c>
       <c r="C2219" t="s">
-        <v>2179</v>
+        <v>2445</v>
       </c>
       <c r="D2219">
         <v>0.0</v>
@@ -102876,10 +102969,10 @@
         <v>2587</v>
       </c>
       <c r="I2219" t="s">
+        <v>2584</v>
+      </c>
+      <c r="J2219" t="s">
         <v>2588</v>
-      </c>
-      <c r="J2219" t="s">
-        <v>2589</v>
       </c>
       <c r="K2219">
         <v>0.0</v>
@@ -102891,37 +102984,37 @@
         <v>2415</v>
       </c>
       <c r="N2219" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="2220" spans="1:15">
       <c r="A2220">
-        <v>77351</v>
+        <v>77354</v>
       </c>
       <c r="B2220">
         <v>101010204</v>
       </c>
       <c r="C2220" t="s">
-        <v>2445</v>
+        <v>2552</v>
       </c>
       <c r="D2220">
-        <v>2334000.0</v>
+        <v>2650000.0</v>
       </c>
       <c r="E2220">
         <v>0.0</v>
       </c>
       <c r="F2220">
-        <v>2334000.0</v>
+        <v>2650000.0</v>
       </c>
       <c r="G2220"/>
       <c r="H2220" t="s">
+        <v>2590</v>
+      </c>
+      <c r="I2220" t="s">
+        <v>246</v>
+      </c>
+      <c r="J2220" t="s">
         <v>2591</v>
-      </c>
-      <c r="I2220" t="s">
-        <v>2588</v>
-      </c>
-      <c r="J2220" t="s">
-        <v>2592</v>
       </c>
       <c r="K2220">
         <v>0.0</v>
@@ -102933,37 +103026,37 @@
         <v>2415</v>
       </c>
       <c r="N2220" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="2221" spans="1:15">
       <c r="A2221">
-        <v>77352</v>
+        <v>77355</v>
       </c>
       <c r="B2221">
         <v>403010100</v>
       </c>
       <c r="C2221" t="s">
-        <v>2445</v>
+        <v>2552</v>
       </c>
       <c r="D2221">
         <v>0.0</v>
       </c>
       <c r="E2221">
-        <v>250000.0</v>
+        <v>150000.0</v>
       </c>
       <c r="F2221">
         <v>0</v>
       </c>
       <c r="G2221"/>
       <c r="H2221" t="s">
+        <v>2590</v>
+      </c>
+      <c r="I2221" t="s">
+        <v>246</v>
+      </c>
+      <c r="J2221" t="s">
         <v>2591</v>
-      </c>
-      <c r="I2221" t="s">
-        <v>2588</v>
-      </c>
-      <c r="J2221" t="s">
-        <v>2592</v>
       </c>
       <c r="K2221">
         <v>0.0</v>
@@ -102975,24 +103068,24 @@
         <v>2415</v>
       </c>
       <c r="N2221" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="2222" spans="1:15">
       <c r="A2222">
-        <v>77353</v>
+        <v>77356</v>
       </c>
       <c r="B2222">
-        <v>101060207</v>
+        <v>101060202</v>
       </c>
       <c r="C2222" t="s">
-        <v>2445</v>
+        <v>2552</v>
       </c>
       <c r="D2222">
         <v>0.0</v>
       </c>
       <c r="E2222">
-        <v>2084000.0</v>
+        <v>2500000.0</v>
       </c>
       <c r="F2222">
         <v>0</v>
@@ -103001,13 +103094,13 @@
         <v>15</v>
       </c>
       <c r="H2222" t="s">
+        <v>2590</v>
+      </c>
+      <c r="I2222" t="s">
+        <v>246</v>
+      </c>
+      <c r="J2222" t="s">
         <v>2591</v>
-      </c>
-      <c r="I2222" t="s">
-        <v>2588</v>
-      </c>
-      <c r="J2222" t="s">
-        <v>2592</v>
       </c>
       <c r="K2222">
         <v>0.0</v>
@@ -103019,37 +103112,37 @@
         <v>2415</v>
       </c>
       <c r="N2222" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="2223" spans="1:15">
       <c r="A2223">
-        <v>77354</v>
+        <v>77357</v>
       </c>
       <c r="B2223">
         <v>101010204</v>
       </c>
       <c r="C2223" t="s">
-        <v>2556</v>
+        <v>2552</v>
       </c>
       <c r="D2223">
-        <v>2650000.0</v>
+        <v>3734000.0</v>
       </c>
       <c r="E2223">
         <v>0.0</v>
       </c>
       <c r="F2223">
-        <v>2650000.0</v>
+        <v>3734000.0</v>
       </c>
       <c r="G2223"/>
       <c r="H2223" t="s">
+        <v>2593</v>
+      </c>
+      <c r="I2223" t="s">
+        <v>255</v>
+      </c>
+      <c r="J2223" t="s">
         <v>2594</v>
-      </c>
-      <c r="I2223" t="s">
-        <v>246</v>
-      </c>
-      <c r="J2223" t="s">
-        <v>2595</v>
       </c>
       <c r="K2223">
         <v>0.0</v>
@@ -103061,37 +103154,37 @@
         <v>2415</v>
       </c>
       <c r="N2223" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="2224" spans="1:15">
       <c r="A2224">
-        <v>77355</v>
+        <v>77358</v>
       </c>
       <c r="B2224">
         <v>403010100</v>
       </c>
       <c r="C2224" t="s">
-        <v>2556</v>
+        <v>2552</v>
       </c>
       <c r="D2224">
         <v>0.0</v>
       </c>
       <c r="E2224">
-        <v>150000.0</v>
+        <v>400000.0</v>
       </c>
       <c r="F2224">
         <v>0</v>
       </c>
       <c r="G2224"/>
       <c r="H2224" t="s">
+        <v>2593</v>
+      </c>
+      <c r="I2224" t="s">
+        <v>255</v>
+      </c>
+      <c r="J2224" t="s">
         <v>2594</v>
-      </c>
-      <c r="I2224" t="s">
-        <v>246</v>
-      </c>
-      <c r="J2224" t="s">
-        <v>2595</v>
       </c>
       <c r="K2224">
         <v>0.0</v>
@@ -103103,24 +103196,24 @@
         <v>2415</v>
       </c>
       <c r="N2224" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="2225" spans="1:15">
       <c r="A2225">
-        <v>77356</v>
+        <v>77359</v>
       </c>
       <c r="B2225">
         <v>101060202</v>
       </c>
       <c r="C2225" t="s">
-        <v>2556</v>
+        <v>2552</v>
       </c>
       <c r="D2225">
         <v>0.0</v>
       </c>
       <c r="E2225">
-        <v>2500000.0</v>
+        <v>3334000.0</v>
       </c>
       <c r="F2225">
         <v>0</v>
@@ -103129,13 +103222,13 @@
         <v>15</v>
       </c>
       <c r="H2225" t="s">
+        <v>2593</v>
+      </c>
+      <c r="I2225" t="s">
+        <v>255</v>
+      </c>
+      <c r="J2225" t="s">
         <v>2594</v>
-      </c>
-      <c r="I2225" t="s">
-        <v>246</v>
-      </c>
-      <c r="J2225" t="s">
-        <v>2595</v>
       </c>
       <c r="K2225">
         <v>0.0</v>
@@ -103147,37 +103240,37 @@
         <v>2415</v>
       </c>
       <c r="N2225" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="2226" spans="1:15">
       <c r="A2226">
-        <v>77357</v>
+        <v>77360</v>
       </c>
       <c r="B2226">
-        <v>101010204</v>
+        <v>101010101</v>
       </c>
       <c r="C2226" t="s">
-        <v>2556</v>
+        <v>2552</v>
       </c>
       <c r="D2226">
-        <v>3734000.0</v>
+        <v>2000000.0</v>
       </c>
       <c r="E2226">
         <v>0.0</v>
       </c>
       <c r="F2226">
-        <v>3734000.0</v>
+        <v>2000000.0</v>
       </c>
       <c r="G2226"/>
       <c r="H2226" t="s">
+        <v>2596</v>
+      </c>
+      <c r="I2226" t="s">
+        <v>388</v>
+      </c>
+      <c r="J2226" t="s">
         <v>2597</v>
-      </c>
-      <c r="I2226" t="s">
-        <v>255</v>
-      </c>
-      <c r="J2226" t="s">
-        <v>2598</v>
       </c>
       <c r="K2226">
         <v>0.0</v>
@@ -103189,37 +103282,37 @@
         <v>2415</v>
       </c>
       <c r="N2226" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="2227" spans="1:15">
       <c r="A2227">
-        <v>77358</v>
+        <v>77361</v>
       </c>
       <c r="B2227">
         <v>403010100</v>
       </c>
       <c r="C2227" t="s">
-        <v>2556</v>
+        <v>2552</v>
       </c>
       <c r="D2227">
         <v>0.0</v>
       </c>
       <c r="E2227">
-        <v>400000.0</v>
+        <v>200000.0</v>
       </c>
       <c r="F2227">
         <v>0</v>
       </c>
       <c r="G2227"/>
       <c r="H2227" t="s">
+        <v>2596</v>
+      </c>
+      <c r="I2227" t="s">
+        <v>388</v>
+      </c>
+      <c r="J2227" t="s">
         <v>2597</v>
-      </c>
-      <c r="I2227" t="s">
-        <v>255</v>
-      </c>
-      <c r="J2227" t="s">
-        <v>2598</v>
       </c>
       <c r="K2227">
         <v>0.0</v>
@@ -103231,24 +103324,24 @@
         <v>2415</v>
       </c>
       <c r="N2227" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="2228" spans="1:15">
       <c r="A2228">
-        <v>77359</v>
+        <v>77362</v>
       </c>
       <c r="B2228">
-        <v>101060202</v>
+        <v>101060207</v>
       </c>
       <c r="C2228" t="s">
-        <v>2556</v>
+        <v>2552</v>
       </c>
       <c r="D2228">
         <v>0.0</v>
       </c>
       <c r="E2228">
-        <v>3334000.0</v>
+        <v>1800000.0</v>
       </c>
       <c r="F2228">
         <v>0</v>
@@ -103257,13 +103350,13 @@
         <v>15</v>
       </c>
       <c r="H2228" t="s">
+        <v>2596</v>
+      </c>
+      <c r="I2228" t="s">
+        <v>388</v>
+      </c>
+      <c r="J2228" t="s">
         <v>2597</v>
-      </c>
-      <c r="I2228" t="s">
-        <v>255</v>
-      </c>
-      <c r="J2228" t="s">
-        <v>2598</v>
       </c>
       <c r="K2228">
         <v>0.0</v>
@@ -103275,34 +103368,34 @@
         <v>2415</v>
       </c>
       <c r="N2228" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="2229" spans="1:15">
       <c r="A2229">
-        <v>77360</v>
+        <v>77394</v>
       </c>
       <c r="B2229">
-        <v>101010101</v>
+        <v>101010204</v>
       </c>
       <c r="C2229" t="s">
-        <v>2556</v>
+        <v>2599</v>
       </c>
       <c r="D2229">
-        <v>2000000.0</v>
+        <v>500000.0</v>
       </c>
       <c r="E2229">
         <v>0.0</v>
       </c>
       <c r="F2229">
-        <v>2000000.0</v>
+        <v>500000.0</v>
       </c>
       <c r="G2229"/>
       <c r="H2229" t="s">
         <v>2600</v>
       </c>
       <c r="I2229" t="s">
-        <v>388</v>
+        <v>109</v>
       </c>
       <c r="J2229" t="s">
         <v>2601</v>
@@ -103314,37 +103407,37 @@
         <v>0.0</v>
       </c>
       <c r="M2229" t="s">
-        <v>2415</v>
+        <v>2602</v>
       </c>
       <c r="N2229" t="s">
-        <v>2602</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="2230" spans="1:15">
       <c r="A2230">
-        <v>77361</v>
+        <v>77395</v>
       </c>
       <c r="B2230">
         <v>403010100</v>
       </c>
       <c r="C2230" t="s">
-        <v>2556</v>
+        <v>2599</v>
       </c>
       <c r="D2230">
         <v>0.0</v>
       </c>
       <c r="E2230">
-        <v>200000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F2230">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G2230"/>
       <c r="H2230" t="s">
         <v>2600</v>
       </c>
       <c r="I2230" t="s">
-        <v>388</v>
+        <v>109</v>
       </c>
       <c r="J2230" t="s">
         <v>2601</v>
@@ -103356,27 +103449,27 @@
         <v>0.0</v>
       </c>
       <c r="M2230" t="s">
-        <v>2415</v>
+        <v>2602</v>
       </c>
       <c r="N2230" t="s">
-        <v>2602</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="2231" spans="1:15">
       <c r="A2231">
-        <v>77362</v>
+        <v>77396</v>
       </c>
       <c r="B2231">
-        <v>101060207</v>
+        <v>101060202</v>
       </c>
       <c r="C2231" t="s">
-        <v>2556</v>
+        <v>2599</v>
       </c>
       <c r="D2231">
         <v>0.0</v>
       </c>
       <c r="E2231">
-        <v>1800000.0</v>
+        <v>500000.0</v>
       </c>
       <c r="F2231">
         <v>0</v>
@@ -103388,7 +103481,7 @@
         <v>2600</v>
       </c>
       <c r="I2231" t="s">
-        <v>388</v>
+        <v>109</v>
       </c>
       <c r="J2231" t="s">
         <v>2601</v>
@@ -103400,21 +103493,21 @@
         <v>0.0</v>
       </c>
       <c r="M2231" t="s">
-        <v>2415</v>
+        <v>2602</v>
       </c>
       <c r="N2231" t="s">
-        <v>2602</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="2232" spans="1:15">
       <c r="A2232">
-        <v>77363</v>
+        <v>77397</v>
       </c>
       <c r="B2232">
         <v>101010204</v>
       </c>
       <c r="C2232" t="s">
-        <v>2603</v>
+        <v>2604</v>
       </c>
       <c r="D2232">
         <v>2500000.0</v>
@@ -103427,13 +103520,13 @@
       </c>
       <c r="G2232"/>
       <c r="H2232" t="s">
-        <v>407</v>
+        <v>2605</v>
       </c>
       <c r="I2232" t="s">
-        <v>2604</v>
+        <v>234</v>
       </c>
       <c r="J2232" t="s">
-        <v>2605</v>
+        <v>2606</v>
       </c>
       <c r="K2232">
         <v>0.0</v>
@@ -103442,54 +103535,1122 @@
         <v>0.0</v>
       </c>
       <c r="M2232" t="s">
-        <v>2415</v>
+        <v>2602</v>
       </c>
       <c r="N2232" t="s">
-        <v>2606</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="2233" spans="1:15">
       <c r="A2233">
-        <v>77364</v>
+        <v>77398</v>
       </c>
       <c r="B2233">
-        <v>103040206</v>
+        <v>403010100</v>
       </c>
       <c r="C2233" t="s">
-        <v>2603</v>
+        <v>2604</v>
       </c>
       <c r="D2233">
         <v>0.0</v>
       </c>
       <c r="E2233">
+        <v>250000.0</v>
+      </c>
+      <c r="F2233">
+        <v>0</v>
+      </c>
+      <c r="G2233"/>
+      <c r="H2233" t="s">
+        <v>2605</v>
+      </c>
+      <c r="I2233" t="s">
+        <v>234</v>
+      </c>
+      <c r="J2233" t="s">
+        <v>2606</v>
+      </c>
+      <c r="K2233">
+        <v>0.0</v>
+      </c>
+      <c r="L2233">
+        <v>0.0</v>
+      </c>
+      <c r="M2233" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2233" t="s">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:15">
+      <c r="A2234">
+        <v>77399</v>
+      </c>
+      <c r="B2234">
+        <v>101060202</v>
+      </c>
+      <c r="C2234" t="s">
+        <v>2604</v>
+      </c>
+      <c r="D2234">
+        <v>0.0</v>
+      </c>
+      <c r="E2234">
+        <v>2250000.0</v>
+      </c>
+      <c r="F2234">
+        <v>0</v>
+      </c>
+      <c r="G2234" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2234" t="s">
+        <v>2605</v>
+      </c>
+      <c r="I2234" t="s">
+        <v>234</v>
+      </c>
+      <c r="J2234" t="s">
+        <v>2606</v>
+      </c>
+      <c r="K2234">
+        <v>0.0</v>
+      </c>
+      <c r="L2234">
+        <v>0.0</v>
+      </c>
+      <c r="M2234" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2234" t="s">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:15">
+      <c r="A2235">
+        <v>77400</v>
+      </c>
+      <c r="B2235">
+        <v>101010204</v>
+      </c>
+      <c r="C2235" t="s">
+        <v>2608</v>
+      </c>
+      <c r="D2235">
+        <v>1105000.0</v>
+      </c>
+      <c r="E2235">
+        <v>0.0</v>
+      </c>
+      <c r="F2235">
+        <v>1105000.0</v>
+      </c>
+      <c r="G2235"/>
+      <c r="H2235" t="s">
+        <v>2609</v>
+      </c>
+      <c r="I2235" t="s">
+        <v>322</v>
+      </c>
+      <c r="J2235" t="s">
+        <v>2610</v>
+      </c>
+      <c r="K2235">
+        <v>0.0</v>
+      </c>
+      <c r="L2235">
+        <v>0.0</v>
+      </c>
+      <c r="M2235" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2235" t="s">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:15">
+      <c r="A2236">
+        <v>77401</v>
+      </c>
+      <c r="B2236">
+        <v>403010100</v>
+      </c>
+      <c r="C2236" t="s">
+        <v>2608</v>
+      </c>
+      <c r="D2236">
+        <v>0.0</v>
+      </c>
+      <c r="E2236">
+        <v>62500.0</v>
+      </c>
+      <c r="F2236">
+        <v>0</v>
+      </c>
+      <c r="G2236"/>
+      <c r="H2236" t="s">
+        <v>2609</v>
+      </c>
+      <c r="I2236" t="s">
+        <v>322</v>
+      </c>
+      <c r="J2236" t="s">
+        <v>2610</v>
+      </c>
+      <c r="K2236">
+        <v>0.0</v>
+      </c>
+      <c r="L2236">
+        <v>0.0</v>
+      </c>
+      <c r="M2236" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2236" t="s">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:15">
+      <c r="A2237">
+        <v>77402</v>
+      </c>
+      <c r="B2237">
+        <v>101060202</v>
+      </c>
+      <c r="C2237" t="s">
+        <v>2608</v>
+      </c>
+      <c r="D2237">
+        <v>0.0</v>
+      </c>
+      <c r="E2237">
+        <v>1042500.0</v>
+      </c>
+      <c r="F2237">
+        <v>0</v>
+      </c>
+      <c r="G2237" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2237" t="s">
+        <v>2609</v>
+      </c>
+      <c r="I2237" t="s">
+        <v>322</v>
+      </c>
+      <c r="J2237" t="s">
+        <v>2610</v>
+      </c>
+      <c r="K2237">
+        <v>0.0</v>
+      </c>
+      <c r="L2237">
+        <v>0.0</v>
+      </c>
+      <c r="M2237" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2237" t="s">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:15">
+      <c r="A2238">
+        <v>77403</v>
+      </c>
+      <c r="B2238">
+        <v>101010204</v>
+      </c>
+      <c r="C2238" t="s">
+        <v>2612</v>
+      </c>
+      <c r="D2238">
+        <v>2650000.0</v>
+      </c>
+      <c r="E2238">
+        <v>0.0</v>
+      </c>
+      <c r="F2238">
+        <v>2650000.0</v>
+      </c>
+      <c r="G2238"/>
+      <c r="H2238" t="s">
+        <v>2613</v>
+      </c>
+      <c r="I2238" t="s">
+        <v>360</v>
+      </c>
+      <c r="J2238" t="s">
+        <v>2614</v>
+      </c>
+      <c r="K2238">
+        <v>0.0</v>
+      </c>
+      <c r="L2238">
+        <v>0.0</v>
+      </c>
+      <c r="M2238" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2238" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:15">
+      <c r="A2239">
+        <v>77404</v>
+      </c>
+      <c r="B2239">
+        <v>403010100</v>
+      </c>
+      <c r="C2239" t="s">
+        <v>2612</v>
+      </c>
+      <c r="D2239">
+        <v>0.0</v>
+      </c>
+      <c r="E2239">
+        <v>150000.0</v>
+      </c>
+      <c r="F2239">
+        <v>0</v>
+      </c>
+      <c r="G2239"/>
+      <c r="H2239" t="s">
+        <v>2613</v>
+      </c>
+      <c r="I2239" t="s">
+        <v>360</v>
+      </c>
+      <c r="J2239" t="s">
+        <v>2614</v>
+      </c>
+      <c r="K2239">
+        <v>0.0</v>
+      </c>
+      <c r="L2239">
+        <v>0.0</v>
+      </c>
+      <c r="M2239" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2239" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:15">
+      <c r="A2240">
+        <v>77405</v>
+      </c>
+      <c r="B2240">
+        <v>101060202</v>
+      </c>
+      <c r="C2240" t="s">
+        <v>2612</v>
+      </c>
+      <c r="D2240">
+        <v>0.0</v>
+      </c>
+      <c r="E2240">
         <v>2500000.0</v>
       </c>
-      <c r="F2233">
-        <v>0</v>
-      </c>
-      <c r="G2233" t="s">
+      <c r="F2240">
+        <v>0</v>
+      </c>
+      <c r="G2240" t="s">
         <v>15</v>
       </c>
-      <c r="H2233" t="s">
-        <v>2607</v>
-      </c>
-      <c r="I2233" t="s">
-        <v>2604</v>
-      </c>
-      <c r="J2233" t="s">
-        <v>2605</v>
-      </c>
-      <c r="K2233">
-        <v>0.0</v>
-      </c>
-      <c r="L2233">
-        <v>0.0</v>
-      </c>
-      <c r="M2233" t="s">
-        <v>2415</v>
-      </c>
-      <c r="N2233" t="s">
-        <v>2606</v>
+      <c r="H2240" t="s">
+        <v>2613</v>
+      </c>
+      <c r="I2240" t="s">
+        <v>360</v>
+      </c>
+      <c r="J2240" t="s">
+        <v>2614</v>
+      </c>
+      <c r="K2240">
+        <v>0.0</v>
+      </c>
+      <c r="L2240">
+        <v>0.0</v>
+      </c>
+      <c r="M2240" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2240" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="2241" spans="1:15">
+      <c r="A2241">
+        <v>77406</v>
+      </c>
+      <c r="B2241">
+        <v>101010204</v>
+      </c>
+      <c r="C2241" t="s">
+        <v>2616</v>
+      </c>
+      <c r="D2241">
+        <v>2250000.0</v>
+      </c>
+      <c r="E2241">
+        <v>0.0</v>
+      </c>
+      <c r="F2241">
+        <v>2250000.0</v>
+      </c>
+      <c r="G2241"/>
+      <c r="H2241" t="s">
+        <v>2617</v>
+      </c>
+      <c r="I2241" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2241" t="s">
+        <v>2618</v>
+      </c>
+      <c r="K2241">
+        <v>0.0</v>
+      </c>
+      <c r="L2241">
+        <v>0.0</v>
+      </c>
+      <c r="M2241" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2241" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="2242" spans="1:15">
+      <c r="A2242">
+        <v>77407</v>
+      </c>
+      <c r="B2242">
+        <v>403010100</v>
+      </c>
+      <c r="C2242" t="s">
+        <v>2616</v>
+      </c>
+      <c r="D2242">
+        <v>0.0</v>
+      </c>
+      <c r="E2242">
+        <v>125000.0</v>
+      </c>
+      <c r="F2242">
+        <v>0</v>
+      </c>
+      <c r="G2242"/>
+      <c r="H2242" t="s">
+        <v>2617</v>
+      </c>
+      <c r="I2242" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2242" t="s">
+        <v>2618</v>
+      </c>
+      <c r="K2242">
+        <v>0.0</v>
+      </c>
+      <c r="L2242">
+        <v>0.0</v>
+      </c>
+      <c r="M2242" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2242" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="2243" spans="1:15">
+      <c r="A2243">
+        <v>77408</v>
+      </c>
+      <c r="B2243">
+        <v>101060202</v>
+      </c>
+      <c r="C2243" t="s">
+        <v>2616</v>
+      </c>
+      <c r="D2243">
+        <v>0.0</v>
+      </c>
+      <c r="E2243">
+        <v>2125000.0</v>
+      </c>
+      <c r="F2243">
+        <v>0</v>
+      </c>
+      <c r="G2243" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2243" t="s">
+        <v>2617</v>
+      </c>
+      <c r="I2243" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2243" t="s">
+        <v>2618</v>
+      </c>
+      <c r="K2243">
+        <v>0.0</v>
+      </c>
+      <c r="L2243">
+        <v>0.0</v>
+      </c>
+      <c r="M2243" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2243" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:15">
+      <c r="A2244">
+        <v>77409</v>
+      </c>
+      <c r="B2244">
+        <v>101010204</v>
+      </c>
+      <c r="C2244" t="s">
+        <v>2620</v>
+      </c>
+      <c r="D2244">
+        <v>2209000.0</v>
+      </c>
+      <c r="E2244">
+        <v>0.0</v>
+      </c>
+      <c r="F2244">
+        <v>2209000.0</v>
+      </c>
+      <c r="G2244"/>
+      <c r="H2244" t="s">
+        <v>2621</v>
+      </c>
+      <c r="I2244" t="s">
+        <v>309</v>
+      </c>
+      <c r="J2244" t="s">
+        <v>2622</v>
+      </c>
+      <c r="K2244">
+        <v>0.0</v>
+      </c>
+      <c r="L2244">
+        <v>0.0</v>
+      </c>
+      <c r="M2244" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2244" t="s">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:15">
+      <c r="A2245">
+        <v>77410</v>
+      </c>
+      <c r="B2245">
+        <v>403010100</v>
+      </c>
+      <c r="C2245" t="s">
+        <v>2620</v>
+      </c>
+      <c r="D2245">
+        <v>0.0</v>
+      </c>
+      <c r="E2245">
+        <v>125000.0</v>
+      </c>
+      <c r="F2245">
+        <v>0</v>
+      </c>
+      <c r="G2245"/>
+      <c r="H2245" t="s">
+        <v>2621</v>
+      </c>
+      <c r="I2245" t="s">
+        <v>309</v>
+      </c>
+      <c r="J2245" t="s">
+        <v>2622</v>
+      </c>
+      <c r="K2245">
+        <v>0.0</v>
+      </c>
+      <c r="L2245">
+        <v>0.0</v>
+      </c>
+      <c r="M2245" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2245" t="s">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:15">
+      <c r="A2246">
+        <v>77411</v>
+      </c>
+      <c r="B2246">
+        <v>101060202</v>
+      </c>
+      <c r="C2246" t="s">
+        <v>2620</v>
+      </c>
+      <c r="D2246">
+        <v>0.0</v>
+      </c>
+      <c r="E2246">
+        <v>2084000.0</v>
+      </c>
+      <c r="F2246">
+        <v>0</v>
+      </c>
+      <c r="G2246" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2246" t="s">
+        <v>2621</v>
+      </c>
+      <c r="I2246" t="s">
+        <v>309</v>
+      </c>
+      <c r="J2246" t="s">
+        <v>2622</v>
+      </c>
+      <c r="K2246">
+        <v>0.0</v>
+      </c>
+      <c r="L2246">
+        <v>0.0</v>
+      </c>
+      <c r="M2246" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2246" t="s">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:15">
+      <c r="A2247">
+        <v>77412</v>
+      </c>
+      <c r="B2247">
+        <v>407010000</v>
+      </c>
+      <c r="C2247" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D2247">
+        <v>200000.0</v>
+      </c>
+      <c r="E2247">
+        <v>0.0</v>
+      </c>
+      <c r="F2247">
+        <v>200000.0</v>
+      </c>
+      <c r="G2247"/>
+      <c r="H2247" t="s">
+        <v>403</v>
+      </c>
+      <c r="I2247" t="s">
+        <v>2624</v>
+      </c>
+      <c r="J2247" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K2247">
+        <v>0.0</v>
+      </c>
+      <c r="L2247">
+        <v>0.0</v>
+      </c>
+      <c r="M2247" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2247" t="s">
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="2248" spans="1:15">
+      <c r="A2248">
+        <v>77413</v>
+      </c>
+      <c r="B2248">
+        <v>101010204</v>
+      </c>
+      <c r="C2248" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D2248">
+        <v>0.0</v>
+      </c>
+      <c r="E2248">
+        <v>200000.0</v>
+      </c>
+      <c r="F2248">
+        <v>0</v>
+      </c>
+      <c r="G2248" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2248" t="s">
+        <v>407</v>
+      </c>
+      <c r="I2248" t="s">
+        <v>2624</v>
+      </c>
+      <c r="J2248" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K2248">
+        <v>0.0</v>
+      </c>
+      <c r="L2248">
+        <v>0.0</v>
+      </c>
+      <c r="M2248" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2248" t="s">
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:15">
+      <c r="A2249">
+        <v>77414</v>
+      </c>
+      <c r="B2249">
+        <v>407010000</v>
+      </c>
+      <c r="C2249" t="s">
+        <v>2576</v>
+      </c>
+      <c r="D2249">
+        <v>87639.0</v>
+      </c>
+      <c r="E2249">
+        <v>0.0</v>
+      </c>
+      <c r="F2249">
+        <v>87639.0</v>
+      </c>
+      <c r="G2249"/>
+      <c r="H2249" t="s">
+        <v>403</v>
+      </c>
+      <c r="I2249" t="s">
+        <v>2627</v>
+      </c>
+      <c r="J2249" t="s">
+        <v>2628</v>
+      </c>
+      <c r="K2249">
+        <v>0.0</v>
+      </c>
+      <c r="L2249">
+        <v>0.0</v>
+      </c>
+      <c r="M2249" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2249" t="s">
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:15">
+      <c r="A2250">
+        <v>77415</v>
+      </c>
+      <c r="B2250">
+        <v>101010204</v>
+      </c>
+      <c r="C2250" t="s">
+        <v>2576</v>
+      </c>
+      <c r="D2250">
+        <v>0.0</v>
+      </c>
+      <c r="E2250">
+        <v>87639.0</v>
+      </c>
+      <c r="F2250">
+        <v>0</v>
+      </c>
+      <c r="G2250" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2250" t="s">
+        <v>407</v>
+      </c>
+      <c r="I2250" t="s">
+        <v>2627</v>
+      </c>
+      <c r="J2250" t="s">
+        <v>2628</v>
+      </c>
+      <c r="K2250">
+        <v>0.0</v>
+      </c>
+      <c r="L2250">
+        <v>0.0</v>
+      </c>
+      <c r="M2250" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2250" t="s">
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:15">
+      <c r="A2251">
+        <v>77418</v>
+      </c>
+      <c r="B2251">
+        <v>101010204</v>
+      </c>
+      <c r="C2251" t="s">
+        <v>2599</v>
+      </c>
+      <c r="D2251">
+        <v>4434000.0</v>
+      </c>
+      <c r="E2251">
+        <v>0.0</v>
+      </c>
+      <c r="F2251">
+        <v>4434000.0</v>
+      </c>
+      <c r="G2251"/>
+      <c r="H2251" t="s">
+        <v>2630</v>
+      </c>
+      <c r="I2251" t="s">
+        <v>326</v>
+      </c>
+      <c r="J2251" t="s">
+        <v>2631</v>
+      </c>
+      <c r="K2251">
+        <v>0.0</v>
+      </c>
+      <c r="L2251">
+        <v>0.0</v>
+      </c>
+      <c r="M2251" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2251" t="s">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:15">
+      <c r="A2252">
+        <v>77419</v>
+      </c>
+      <c r="B2252">
+        <v>403010100</v>
+      </c>
+      <c r="C2252" t="s">
+        <v>2599</v>
+      </c>
+      <c r="D2252">
+        <v>0.0</v>
+      </c>
+      <c r="E2252">
+        <v>475000.0</v>
+      </c>
+      <c r="F2252">
+        <v>0</v>
+      </c>
+      <c r="G2252"/>
+      <c r="H2252" t="s">
+        <v>2630</v>
+      </c>
+      <c r="I2252" t="s">
+        <v>326</v>
+      </c>
+      <c r="J2252" t="s">
+        <v>2631</v>
+      </c>
+      <c r="K2252">
+        <v>0.0</v>
+      </c>
+      <c r="L2252">
+        <v>0.0</v>
+      </c>
+      <c r="M2252" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2252" t="s">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:15">
+      <c r="A2253">
+        <v>77420</v>
+      </c>
+      <c r="B2253">
+        <v>101060207</v>
+      </c>
+      <c r="C2253" t="s">
+        <v>2599</v>
+      </c>
+      <c r="D2253">
+        <v>0.0</v>
+      </c>
+      <c r="E2253">
+        <v>3959000.0</v>
+      </c>
+      <c r="F2253">
+        <v>0</v>
+      </c>
+      <c r="G2253" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2253" t="s">
+        <v>2630</v>
+      </c>
+      <c r="I2253" t="s">
+        <v>326</v>
+      </c>
+      <c r="J2253" t="s">
+        <v>2631</v>
+      </c>
+      <c r="K2253">
+        <v>0.0</v>
+      </c>
+      <c r="L2253">
+        <v>0.0</v>
+      </c>
+      <c r="M2253" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2253" t="s">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:15">
+      <c r="A2254">
+        <v>77421</v>
+      </c>
+      <c r="B2254">
+        <v>101010204</v>
+      </c>
+      <c r="C2254" t="s">
+        <v>2576</v>
+      </c>
+      <c r="D2254">
+        <v>430697.0</v>
+      </c>
+      <c r="E2254">
+        <v>0.0</v>
+      </c>
+      <c r="F2254">
+        <v>430697.0</v>
+      </c>
+      <c r="G2254"/>
+      <c r="H2254" t="s">
+        <v>407</v>
+      </c>
+      <c r="I2254" t="s">
+        <v>2633</v>
+      </c>
+      <c r="J2254" t="s">
+        <v>2634</v>
+      </c>
+      <c r="K2254">
+        <v>0.0</v>
+      </c>
+      <c r="L2254">
+        <v>0.0</v>
+      </c>
+      <c r="M2254" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2254" t="s">
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:15">
+      <c r="A2255">
+        <v>77422</v>
+      </c>
+      <c r="B2255">
+        <v>403020100</v>
+      </c>
+      <c r="C2255" t="s">
+        <v>2576</v>
+      </c>
+      <c r="D2255">
+        <v>0.0</v>
+      </c>
+      <c r="E2255">
+        <v>430697.0</v>
+      </c>
+      <c r="F2255">
+        <v>0</v>
+      </c>
+      <c r="G2255" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2255" t="s">
+        <v>406</v>
+      </c>
+      <c r="I2255" t="s">
+        <v>2633</v>
+      </c>
+      <c r="J2255" t="s">
+        <v>2634</v>
+      </c>
+      <c r="K2255">
+        <v>0.0</v>
+      </c>
+      <c r="L2255">
+        <v>0.0</v>
+      </c>
+      <c r="M2255" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2255" t="s">
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:15">
+      <c r="A2256">
+        <v>77423</v>
+      </c>
+      <c r="B2256">
+        <v>101010101</v>
+      </c>
+      <c r="C2256" t="s">
+        <v>677</v>
+      </c>
+      <c r="D2256">
+        <v>1000000.0</v>
+      </c>
+      <c r="E2256">
+        <v>0.0</v>
+      </c>
+      <c r="F2256">
+        <v>1000000.0</v>
+      </c>
+      <c r="G2256"/>
+      <c r="H2256" t="s">
+        <v>2636</v>
+      </c>
+      <c r="I2256" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2256" t="s">
+        <v>2637</v>
+      </c>
+      <c r="K2256">
+        <v>0.0</v>
+      </c>
+      <c r="L2256">
+        <v>0.0</v>
+      </c>
+      <c r="M2256" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2256" t="s">
+        <v>2638</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:15">
+      <c r="A2257">
+        <v>77424</v>
+      </c>
+      <c r="B2257">
+        <v>403010100</v>
+      </c>
+      <c r="C2257" t="s">
+        <v>677</v>
+      </c>
+      <c r="D2257">
+        <v>0.0</v>
+      </c>
+      <c r="E2257">
+        <v>183332.0</v>
+      </c>
+      <c r="F2257">
+        <v>0</v>
+      </c>
+      <c r="G2257"/>
+      <c r="H2257" t="s">
+        <v>2636</v>
+      </c>
+      <c r="I2257" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2257" t="s">
+        <v>2637</v>
+      </c>
+      <c r="K2257">
+        <v>0.0</v>
+      </c>
+      <c r="L2257">
+        <v>0.0</v>
+      </c>
+      <c r="M2257" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2257" t="s">
+        <v>2638</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:15">
+      <c r="A2258">
+        <v>77425</v>
+      </c>
+      <c r="B2258">
+        <v>101060202</v>
+      </c>
+      <c r="C2258" t="s">
+        <v>677</v>
+      </c>
+      <c r="D2258">
+        <v>0.0</v>
+      </c>
+      <c r="E2258">
+        <v>816668.0</v>
+      </c>
+      <c r="F2258">
+        <v>0</v>
+      </c>
+      <c r="G2258" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2258" t="s">
+        <v>2636</v>
+      </c>
+      <c r="I2258" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2258" t="s">
+        <v>2637</v>
+      </c>
+      <c r="K2258">
+        <v>0.0</v>
+      </c>
+      <c r="L2258">
+        <v>0.0</v>
+      </c>
+      <c r="M2258" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N2258" t="s">
+        <v>2638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>